<commit_message>
226, 241 v2, add good, bad number, remove first norm for le, add 226 info, change 241 date, add code to plot the bubble plot to run.m
</commit_message>
<xml_diff>
--- a/num_point_report.xlsx
+++ b/num_point_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hp/GitHub/EEG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC3248B-22BF-604C-91F3-2CB52EF16A14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C525B0-0CA9-7448-BA11-431DABBE293D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{CC2A87F3-E22E-E243-B7CE-7680353FEA94}"/>
+    <workbookView xWindow="5640" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{CC2A87F3-E22E-E243-B7CE-7680353FEA94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,40 +25,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>Patient 231</t>
-  </si>
-  <si>
-    <t>Patient 222</t>
-  </si>
-  <si>
-    <t>Total dat file</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Scheduled </t>
   </si>
   <si>
-    <t>Patient 222_1</t>
-  </si>
-  <si>
-    <t>Patient 222_2</t>
-  </si>
-  <si>
-    <t>Patient 222_3</t>
-  </si>
-  <si>
     <t>good</t>
   </si>
   <si>
     <t>bad</t>
+  </si>
+  <si>
+    <t>222_1</t>
+  </si>
+  <si>
+    <t>222_2</t>
+  </si>
+  <si>
+    <t>222_3</t>
+  </si>
+  <si>
+    <t>patient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -403,84 +397,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AF7602-22BA-E34F-B8A8-3A7E7F4DD39D}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>231</v>
+      </c>
+      <c r="F1">
+        <v>229</v>
+      </c>
+      <c r="G1">
+        <v>241</v>
+      </c>
+      <c r="H1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>728</v>
+      </c>
+      <c r="C2">
+        <v>624</v>
+      </c>
+      <c r="D2">
+        <v>367</v>
+      </c>
+      <c r="E2">
+        <v>893</v>
+      </c>
+      <c r="F2">
+        <v>1115</v>
+      </c>
+      <c r="G2">
+        <v>569</v>
+      </c>
+      <c r="H2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
+      <c r="B3">
+        <v>276</v>
+      </c>
+      <c r="C3">
+        <v>265</v>
+      </c>
+      <c r="D3">
+        <v>185</v>
+      </c>
+      <c r="E3">
+        <v>537</v>
+      </c>
+      <c r="F3">
+        <v>346</v>
+      </c>
+      <c r="G3">
+        <v>288</v>
+      </c>
+      <c r="H3">
+        <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>3342</v>
-      </c>
-      <c r="C2">
-        <v>2608</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>55</v>
-      </c>
-      <c r="G2">
-        <v>32</v>
-      </c>
-      <c r="H2">
-        <v>37</v>
-      </c>
-      <c r="I2">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>506</v>
-      </c>
-      <c r="C3">
-        <v>650</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>85</v>
-      </c>
-      <c r="G3">
-        <v>76</v>
-      </c>
-      <c r="H3">
-        <v>32</v>
-      </c>
-      <c r="I3">
-        <v>116</v>
+      <c r="B4">
+        <v>452</v>
+      </c>
+      <c r="C4">
+        <v>359</v>
+      </c>
+      <c r="D4">
+        <v>182</v>
+      </c>
+      <c r="E4">
+        <v>356</v>
+      </c>
+      <c r="F4">
+        <v>769</v>
+      </c>
+      <c r="G4">
+        <v>269</v>
+      </c>
+      <c r="H4">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>